<commit_message>
Fixed metadata parse test
</commit_message>
<xml_diff>
--- a/src/main/resources/metadataTestFile.xlsx
+++ b/src/main/resources/metadataTestFile.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Age</t>
   </si>
   <si>
     <t>HIV Status</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Specimen Type</t>
@@ -41,19 +38,7 @@
     <t>Study Geographic District</t>
   </si>
   <si>
-    <t>LAM4</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Specimen ID</t>
-  </si>
-  <si>
-    <t>TKK-01-0001</t>
   </si>
   <si>
     <t>Sex</t>
@@ -92,9 +77,6 @@
     <t>Microscopy Smear Status</t>
   </si>
   <si>
-    <t>MDR</t>
-  </si>
-  <si>
     <t>Date of Collection</t>
   </si>
   <si>
@@ -113,9 +95,6 @@
     <t>DNA isolation: single colony or non-single colony</t>
   </si>
   <si>
-    <t>single colony</t>
-  </si>
-  <si>
     <t>Tugela Ferry vs. non-Tugela Ferry XDR</t>
   </si>
   <si>
@@ -125,16 +104,10 @@
     <t>TKKa</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
     <t>e</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t>f</t>
@@ -147,6 +120,51 @@
   </si>
   <si>
     <t>j</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -878,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA554"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -912,168 +930,168 @@
   <sheetData>
     <row r="1" spans="1:27" s="3" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="O1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>25</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
+      <c r="B2" s="9">
+        <v>1</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
+      <c r="Y2" s="11" t="s">
+        <v>45</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>9</v>
-      </c>
       <c r="AA2" s="8" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>